<commit_message>
Fraz. pluricandidature nel file excel
</commit_message>
<xml_diff>
--- a/dati_2023/dati_2023.xlsx
+++ b/dati_2023/dati_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FC607E-9C8D-44CE-ADDF-455D1E385A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A09DA51-EACA-453B-90CF-AB87251AFD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>LISTA</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>FRAZ_UNI</t>
+  </si>
+  <si>
+    <t>FRAZ_PLURICAND</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,9 +445,10 @@
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +464,11 @@
       <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -477,8 +484,11 @@
       <c r="E2" s="1">
         <v>0.23300000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -494,8 +504,11 @@
       <c r="E3" s="1">
         <v>0.22800000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -511,8 +524,11 @@
       <c r="E4" s="1">
         <v>0.14699999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -528,8 +544,11 @@
       <c r="E5" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -545,8 +564,11 @@
       <c r="E6" s="1">
         <v>9.4E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -562,8 +584,11 @@
       <c r="E7" s="1">
         <v>5.1999999999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -579,8 +604,11 @@
       <c r="E8" s="1">
         <v>2.9000000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -593,8 +621,11 @@
       <c r="E9" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -610,8 +641,11 @@
       <c r="E10" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -624,8 +658,11 @@
       <c r="E11" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -638,8 +675,11 @@
       <c r="E12" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -652,8 +692,11 @@
       <c r="E13" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -666,8 +709,11 @@
       <c r="E14" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -679,6 +725,9 @@
       </c>
       <c r="E15" s="1">
         <v>1.6E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>